<commit_message>
updated succes parsing function and xlxs files
</commit_message>
<xml_diff>
--- a/backend/db/generator/preklad krajin .xlsx
+++ b/backend/db/generator/preklad krajin .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Slavo\Desktop\tis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2F88CD-5C0B-4F56-8251-30372E66FD86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9675093-C53D-4A60-BC3D-FEE296A9EE4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-39540" yWindow="5910" windowWidth="21600" windowHeight="11385" xr2:uid="{46C41BA9-1ED5-4523-8C6C-3A06723AED10}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{46C41BA9-1ED5-4523-8C6C-3A06723AED10}"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
@@ -1137,9 +1137,6 @@
     <t>BURUNDI</t>
   </si>
   <si>
-    <t>CABO VERDE</t>
-  </si>
-  <si>
     <t>CAMBODIA</t>
   </si>
   <si>
@@ -2082,9 +2079,6 @@
     <t>Britské Územie Indického Oceánu</t>
   </si>
   <si>
-    <t>Cabo Verde</t>
-  </si>
-  <si>
     <t>Kajmanské Ostrovy</t>
   </si>
   <si>
@@ -2196,21 +2190,12 @@
     <t>Wallis A Futuna</t>
   </si>
   <si>
-    <t>CONGO, DR</t>
-  </si>
-  <si>
-    <t>CÔTE D'IVOIRE</t>
-  </si>
-  <si>
     <t>FALKLAND ISLANDS (MALVINAS)</t>
   </si>
   <si>
     <t>KOREA DPR</t>
   </si>
   <si>
-    <t>SYRIAN ARAB REPUBLIC</t>
-  </si>
-  <si>
     <t>UNITED KINGDOM</t>
   </si>
   <si>
@@ -2281,6 +2266,21 @@
   </si>
   <si>
     <t>Kórejská republika</t>
+  </si>
+  <si>
+    <t>IVORY COAST</t>
+  </si>
+  <si>
+    <t>SYRIA</t>
+  </si>
+  <si>
+    <t>CONGO DR</t>
+  </si>
+  <si>
+    <t>CAPE VERDE</t>
+  </si>
+  <si>
+    <t>Cape Verde</t>
   </si>
 </sst>
 </file>
@@ -2679,8 +2679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2365B466-160A-4ED5-9BE7-A787968927CB}">
   <dimension ref="A1:G250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="B119" sqref="B119"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2692,10 +2692,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>91</v>
@@ -2710,7 +2710,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>339</v>
@@ -2746,7 +2746,7 @@
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>340</v>
@@ -2764,7 +2764,7 @@
     </row>
     <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>341</v>
@@ -2782,7 +2782,7 @@
     </row>
     <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>342</v>
@@ -2796,7 +2796,7 @@
     </row>
     <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>343</v>
@@ -2814,7 +2814,7 @@
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>344</v>
@@ -2832,7 +2832,7 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>345</v>
@@ -2850,7 +2850,7 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>346</v>
@@ -2868,7 +2868,7 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>45</v>
@@ -2886,7 +2886,7 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>347</v>
@@ -2904,7 +2904,7 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>348</v>
@@ -2958,7 +2958,7 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>349</v>
@@ -2976,7 +2976,7 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>350</v>
@@ -2994,7 +2994,7 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>351</v>
@@ -3003,7 +3003,7 @@
         <v>108</v>
       </c>
       <c r="F18" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
@@ -3012,7 +3012,7 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>352</v>
@@ -3030,7 +3030,7 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>353</v>
@@ -3048,7 +3048,7 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>354</v>
@@ -3084,7 +3084,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>355</v>
@@ -3102,7 +3102,7 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>356</v>
@@ -3120,7 +3120,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>357</v>
@@ -3138,7 +3138,7 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>358</v>
@@ -3147,7 +3147,7 @@
         <v>116</v>
       </c>
       <c r="F26" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="0"/>
@@ -3156,10 +3156,10 @@
     </row>
     <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>117</v>
@@ -3174,7 +3174,7 @@
     </row>
     <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>359</v>
@@ -3192,7 +3192,7 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>360</v>
@@ -3210,7 +3210,7 @@
     </row>
     <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>361</v>
@@ -3228,7 +3228,7 @@
     </row>
     <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>362</v>
@@ -3246,7 +3246,7 @@
     </row>
     <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>48</v>
@@ -3264,7 +3264,7 @@
     </row>
     <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>363</v>
@@ -3282,7 +3282,7 @@
     </row>
     <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>364</v>
@@ -3318,7 +3318,7 @@
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>365</v>
@@ -3336,7 +3336,7 @@
     </row>
     <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>366</v>
@@ -3354,10 +3354,10 @@
     </row>
     <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>682</v>
+        <v>748</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>367</v>
+        <v>747</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>128</v>
@@ -3372,10 +3372,10 @@
     </row>
     <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>129</v>
@@ -3390,16 +3390,16 @@
     </row>
     <row r="40" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>130</v>
       </c>
       <c r="F40" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" si="0"/>
@@ -3426,10 +3426,10 @@
     </row>
     <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>132</v>
@@ -3444,16 +3444,16 @@
     </row>
     <row r="43" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>133</v>
       </c>
       <c r="F43" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="0"/>
@@ -3462,10 +3462,10 @@
     </row>
     <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>134</v>
@@ -3498,7 +3498,7 @@
     </row>
     <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>51</v>
@@ -3516,10 +3516,10 @@
     </row>
     <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>137</v>
@@ -3534,10 +3534,10 @@
     </row>
     <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>138</v>
@@ -3552,10 +3552,10 @@
     </row>
     <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>139</v>
@@ -3570,10 +3570,10 @@
     </row>
     <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>140</v>
@@ -3588,10 +3588,10 @@
     </row>
     <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>141</v>
@@ -3606,10 +3606,10 @@
     </row>
     <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>720</v>
+        <v>746</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>142</v>
@@ -3621,10 +3621,10 @@
     </row>
     <row r="53" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>143</v>
@@ -3636,10 +3636,10 @@
     </row>
     <row r="54" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>144</v>
@@ -3651,10 +3651,10 @@
     </row>
     <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>721</v>
+        <v>744</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>145</v>
@@ -3696,10 +3696,10 @@
     </row>
     <row r="58" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>148</v>
@@ -3711,10 +3711,10 @@
     </row>
     <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>149</v>
@@ -3756,10 +3756,10 @@
     </row>
     <row r="62" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>152</v>
@@ -3771,10 +3771,10 @@
     </row>
     <row r="63" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>153</v>
@@ -3786,10 +3786,10 @@
     </row>
     <row r="64" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>154</v>
@@ -3801,10 +3801,10 @@
     </row>
     <row r="65" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>155</v>
@@ -3816,10 +3816,10 @@
     </row>
     <row r="66" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>156</v>
@@ -3831,10 +3831,10 @@
     </row>
     <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>157</v>
@@ -3846,10 +3846,10 @@
     </row>
     <row r="68" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>158</v>
@@ -3861,10 +3861,10 @@
     </row>
     <row r="69" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>159</v>
@@ -3891,10 +3891,10 @@
     </row>
     <row r="71" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>161</v>
@@ -3906,10 +3906,10 @@
     </row>
     <row r="72" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>162</v>
@@ -3921,10 +3921,10 @@
     </row>
     <row r="73" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>163</v>
@@ -3936,10 +3936,10 @@
     </row>
     <row r="74" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>164</v>
@@ -3951,10 +3951,10 @@
     </row>
     <row r="75" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>165</v>
@@ -3996,10 +3996,10 @@
     </row>
     <row r="78" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>168</v>
@@ -4011,10 +4011,10 @@
     </row>
     <row r="79" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>169</v>
@@ -4026,10 +4026,10 @@
     </row>
     <row r="80" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>170</v>
@@ -4041,10 +4041,10 @@
     </row>
     <row r="81" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>171</v>
@@ -4056,10 +4056,10 @@
     </row>
     <row r="82" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>172</v>
@@ -4071,10 +4071,10 @@
     </row>
     <row r="83" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>173</v>
@@ -4101,10 +4101,10 @@
     </row>
     <row r="85" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>175</v>
@@ -4116,10 +4116,10 @@
     </row>
     <row r="86" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>176</v>
@@ -4146,10 +4146,10 @@
     </row>
     <row r="88" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>178</v>
@@ -4161,10 +4161,10 @@
     </row>
     <row r="89" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>179</v>
@@ -4176,10 +4176,10 @@
     </row>
     <row r="90" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>180</v>
@@ -4191,10 +4191,10 @@
     </row>
     <row r="91" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>181</v>
@@ -4206,10 +4206,10 @@
     </row>
     <row r="92" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>182</v>
@@ -4221,10 +4221,10 @@
     </row>
     <row r="93" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>183</v>
@@ -4236,10 +4236,10 @@
     </row>
     <row r="94" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>184</v>
@@ -4251,10 +4251,10 @@
     </row>
     <row r="95" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>185</v>
@@ -4266,10 +4266,10 @@
     </row>
     <row r="96" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>186</v>
@@ -4281,10 +4281,10 @@
     </row>
     <row r="97" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>187</v>
@@ -4296,10 +4296,10 @@
     </row>
     <row r="98" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>188</v>
@@ -4311,10 +4311,10 @@
     </row>
     <row r="99" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>189</v>
@@ -4326,10 +4326,10 @@
     </row>
     <row r="100" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>190</v>
@@ -4341,10 +4341,10 @@
     </row>
     <row r="101" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>191</v>
@@ -4401,10 +4401,10 @@
     </row>
     <row r="105" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>195</v>
@@ -4419,7 +4419,7 @@
         <v>14</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>196</v>
@@ -4431,10 +4431,10 @@
     </row>
     <row r="107" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>197</v>
@@ -4461,10 +4461,10 @@
     </row>
     <row r="109" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>199</v>
@@ -4506,10 +4506,10 @@
     </row>
     <row r="112" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>202</v>
@@ -4536,10 +4536,10 @@
     </row>
     <row r="114" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>204</v>
@@ -4551,10 +4551,10 @@
     </row>
     <row r="115" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>205</v>
@@ -4566,10 +4566,10 @@
     </row>
     <row r="116" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>206</v>
@@ -4596,10 +4596,10 @@
     </row>
     <row r="118" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>208</v>
@@ -4611,10 +4611,10 @@
     </row>
     <row r="119" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>209</v>
@@ -4626,10 +4626,10 @@
     </row>
     <row r="120" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>748</v>
+        <v>743</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>210</v>
@@ -4641,13 +4641,13 @@
     </row>
     <row r="121" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="G121" t="str">
         <f t="shared" si="1"/>
@@ -4656,10 +4656,10 @@
     </row>
     <row r="122" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>211</v>
@@ -4671,10 +4671,10 @@
     </row>
     <row r="123" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>212</v>
@@ -4686,10 +4686,10 @@
     </row>
     <row r="124" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>213</v>
@@ -4716,10 +4716,10 @@
     </row>
     <row r="126" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>215</v>
@@ -4731,10 +4731,10 @@
     </row>
     <row r="127" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>216</v>
@@ -4746,10 +4746,10 @@
     </row>
     <row r="128" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>217</v>
@@ -4761,10 +4761,10 @@
     </row>
     <row r="129" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>218</v>
@@ -4776,10 +4776,10 @@
     </row>
     <row r="130" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>219</v>
@@ -4821,10 +4821,10 @@
     </row>
     <row r="133" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>222</v>
@@ -4836,10 +4836,10 @@
     </row>
     <row r="134" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C134" s="1" t="s">
         <v>223</v>
@@ -4851,10 +4851,10 @@
     </row>
     <row r="135" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C135" s="1" t="s">
         <v>224</v>
@@ -4866,10 +4866,10 @@
     </row>
     <row r="136" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C136" s="1" t="s">
         <v>225</v>
@@ -4881,10 +4881,10 @@
     </row>
     <row r="137" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C137" s="1" t="s">
         <v>226</v>
@@ -4896,10 +4896,10 @@
     </row>
     <row r="138" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C138" s="1" t="s">
         <v>227</v>
@@ -4911,10 +4911,10 @@
     </row>
     <row r="139" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>228</v>
@@ -4926,10 +4926,10 @@
     </row>
     <row r="140" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C140" s="1" t="s">
         <v>229</v>
@@ -4941,10 +4941,10 @@
     </row>
     <row r="141" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>230</v>
@@ -4956,10 +4956,10 @@
     </row>
     <row r="142" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C142" s="1" t="s">
         <v>231</v>
@@ -4971,10 +4971,10 @@
     </row>
     <row r="143" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C143" s="1" t="s">
         <v>232</v>
@@ -4986,10 +4986,10 @@
     </row>
     <row r="144" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C144" s="1" t="s">
         <v>233</v>
@@ -5016,10 +5016,10 @@
     </row>
     <row r="146" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C146" s="1" t="s">
         <v>235</v>
@@ -5031,10 +5031,10 @@
     </row>
     <row r="147" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C147" s="1" t="s">
         <v>236</v>
@@ -5046,10 +5046,10 @@
     </row>
     <row r="148" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C148" s="1" t="s">
         <v>237</v>
@@ -5061,10 +5061,10 @@
     </row>
     <row r="149" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C149" s="1" t="s">
         <v>238</v>
@@ -5076,10 +5076,10 @@
     </row>
     <row r="150" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C150" s="1" t="s">
         <v>239</v>
@@ -5091,10 +5091,10 @@
     </row>
     <row r="151" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C151" s="1" t="s">
         <v>240</v>
@@ -5106,10 +5106,10 @@
     </row>
     <row r="152" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C152" s="1" t="s">
         <v>241</v>
@@ -5121,10 +5121,10 @@
     </row>
     <row r="153" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C153" s="1" t="s">
         <v>242</v>
@@ -5136,10 +5136,10 @@
     </row>
     <row r="154" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C154" s="1" t="s">
         <v>243</v>
@@ -5151,10 +5151,10 @@
     </row>
     <row r="155" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C155" s="1" t="s">
         <v>244</v>
@@ -5166,10 +5166,10 @@
     </row>
     <row r="156" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C156" s="1" t="s">
         <v>245</v>
@@ -5181,10 +5181,10 @@
     </row>
     <row r="157" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C157" s="1" t="s">
         <v>246</v>
@@ -5211,10 +5211,10 @@
     </row>
     <row r="159" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C159" s="1" t="s">
         <v>248</v>
@@ -5241,10 +5241,10 @@
     </row>
     <row r="161" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C161" s="1" t="s">
         <v>250</v>
@@ -5256,10 +5256,10 @@
     </row>
     <row r="162" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C162" s="1" t="s">
         <v>251</v>
@@ -5271,10 +5271,10 @@
     </row>
     <row r="163" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C163" s="1" t="s">
         <v>252</v>
@@ -5286,10 +5286,10 @@
     </row>
     <row r="164" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C164" s="1" t="s">
         <v>253</v>
@@ -5301,10 +5301,10 @@
     </row>
     <row r="165" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C165" s="1" t="s">
         <v>254</v>
@@ -5316,10 +5316,10 @@
     </row>
     <row r="166" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C166" s="1" t="s">
         <v>255</v>
@@ -5331,10 +5331,10 @@
     </row>
     <row r="167" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="3" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C167" s="1" t="s">
         <v>256</v>
@@ -5361,10 +5361,10 @@
     </row>
     <row r="169" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C169" s="1" t="s">
         <v>258</v>
@@ -5376,10 +5376,10 @@
     </row>
     <row r="170" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C170" s="1" t="s">
         <v>259</v>
@@ -5391,10 +5391,10 @@
     </row>
     <row r="171" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>260</v>
@@ -5406,10 +5406,10 @@
     </row>
     <row r="172" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C172" s="1" t="s">
         <v>261</v>
@@ -5421,10 +5421,10 @@
     </row>
     <row r="173" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>262</v>
@@ -5436,10 +5436,10 @@
     </row>
     <row r="174" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A174" s="3" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C174" s="1" t="s">
         <v>263</v>
@@ -5451,10 +5451,10 @@
     </row>
     <row r="175" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C175" s="1" t="s">
         <v>264</v>
@@ -5466,10 +5466,10 @@
     </row>
     <row r="176" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>265</v>
@@ -5481,10 +5481,10 @@
     </row>
     <row r="177" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C177" s="1" t="s">
         <v>266</v>
@@ -5496,10 +5496,10 @@
     </row>
     <row r="178" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C178" s="1" t="s">
         <v>267</v>
@@ -5541,10 +5541,10 @@
     </row>
     <row r="181" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C181" s="1" t="s">
         <v>270</v>
@@ -5556,10 +5556,10 @@
     </row>
     <row r="182" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C182" s="1" t="s">
         <v>271</v>
@@ -5571,10 +5571,10 @@
     </row>
     <row r="183" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C183" s="1" t="s">
         <v>272</v>
@@ -5604,7 +5604,7 @@
         <v>34</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C185" s="1" t="s">
         <v>274</v>
@@ -5616,10 +5616,10 @@
     </row>
     <row r="186" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>275</v>
@@ -5631,10 +5631,10 @@
     </row>
     <row r="187" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="3" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C187" s="1" t="s">
         <v>276</v>
@@ -5646,10 +5646,10 @@
     </row>
     <row r="188" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A188" s="3" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C188" s="1" t="s">
         <v>277</v>
@@ -5661,10 +5661,10 @@
     </row>
     <row r="189" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="3" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C189" s="1" t="s">
         <v>278</v>
@@ -5676,10 +5676,10 @@
     </row>
     <row r="190" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C190" s="1" t="s">
         <v>279</v>
@@ -5691,10 +5691,10 @@
     </row>
     <row r="191" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="3" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C191" s="1" t="s">
         <v>280</v>
@@ -5706,10 +5706,10 @@
     </row>
     <row r="192" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A192" s="3" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C192" s="1" t="s">
         <v>281</v>
@@ -5721,10 +5721,10 @@
     </row>
     <row r="193" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="3" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C193" s="1" t="s">
         <v>282</v>
@@ -5736,10 +5736,10 @@
     </row>
     <row r="194" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C194" s="1" t="s">
         <v>283</v>
@@ -5751,10 +5751,10 @@
     </row>
     <row r="195" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C195" s="1" t="s">
         <v>284</v>
@@ -5766,10 +5766,10 @@
     </row>
     <row r="196" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A196" s="3" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C196" s="1" t="s">
         <v>285</v>
@@ -5781,10 +5781,10 @@
     </row>
     <row r="197" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C197" s="1" t="s">
         <v>286</v>
@@ -5796,10 +5796,10 @@
     </row>
     <row r="198" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C198" s="1" t="s">
         <v>287</v>
@@ -5826,10 +5826,10 @@
     </row>
     <row r="200" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C200" s="1" t="s">
         <v>289</v>
@@ -5841,10 +5841,10 @@
     </row>
     <row r="201" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C201" s="1" t="s">
         <v>290</v>
@@ -5856,10 +5856,10 @@
     </row>
     <row r="202" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C202" s="1" t="s">
         <v>291</v>
@@ -5871,10 +5871,10 @@
     </row>
     <row r="203" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="3" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C203" s="1" t="s">
         <v>292</v>
@@ -5916,10 +5916,10 @@
     </row>
     <row r="206" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="3" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="B206" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C206" s="1" t="s">
         <v>295</v>
@@ -5931,10 +5931,10 @@
     </row>
     <row r="207" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="B207" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C207" s="1" t="s">
         <v>296</v>
@@ -5946,7 +5946,7 @@
     </row>
     <row r="208" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>65</v>
@@ -5961,10 +5961,10 @@
     </row>
     <row r="209" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A209" s="3" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="B209" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C209" s="1" t="s">
         <v>298</v>
@@ -5976,10 +5976,10 @@
     </row>
     <row r="210" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="B210" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C210" s="1" t="s">
         <v>299</v>
@@ -6006,10 +6006,10 @@
     </row>
     <row r="212" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="B212" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C212" s="1" t="s">
         <v>301</v>
@@ -6021,10 +6021,10 @@
     </row>
     <row r="213" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B213" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C213" s="1" t="s">
         <v>302</v>
@@ -6036,10 +6036,10 @@
     </row>
     <row r="214" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="B214" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C214" s="1" t="s">
         <v>303</v>
@@ -6051,10 +6051,10 @@
     </row>
     <row r="215" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="3" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="B215" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C215" s="1" t="s">
         <v>304</v>
@@ -6096,10 +6096,10 @@
     </row>
     <row r="218" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B218" s="1" t="s">
-        <v>724</v>
+        <v>745</v>
       </c>
       <c r="C218" s="1" t="s">
         <v>307</v>
@@ -6111,10 +6111,10 @@
     </row>
     <row r="219" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B219" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C219" s="1" t="s">
         <v>308</v>
@@ -6126,10 +6126,10 @@
     </row>
     <row r="220" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="B220" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C220" s="1" t="s">
         <v>309</v>
@@ -6141,10 +6141,10 @@
     </row>
     <row r="221" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="B221" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C221" s="1" t="s">
         <v>310</v>
@@ -6156,10 +6156,10 @@
     </row>
     <row r="222" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C222" s="1" t="s">
         <v>311</v>
@@ -6171,10 +6171,10 @@
     </row>
     <row r="223" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C223" s="1" t="s">
         <v>312</v>
@@ -6186,10 +6186,10 @@
     </row>
     <row r="224" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C224" s="1" t="s">
         <v>313</v>
@@ -6201,10 +6201,10 @@
     </row>
     <row r="225" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C225" s="1" t="s">
         <v>314</v>
@@ -6216,10 +6216,10 @@
     </row>
     <row r="226" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C226" s="1" t="s">
         <v>315</v>
@@ -6231,10 +6231,10 @@
     </row>
     <row r="227" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="3" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C227" s="1" t="s">
         <v>316</v>
@@ -6246,10 +6246,10 @@
     </row>
     <row r="228" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C228" s="1" t="s">
         <v>317</v>
@@ -6276,10 +6276,10 @@
     </row>
     <row r="230" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C230" s="1" t="s">
         <v>319</v>
@@ -6291,10 +6291,10 @@
     </row>
     <row r="231" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A231" s="3" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>320</v>
@@ -6306,10 +6306,10 @@
     </row>
     <row r="232" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>321</v>
@@ -6321,10 +6321,10 @@
     </row>
     <row r="233" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" s="2" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>322</v>
@@ -6351,10 +6351,10 @@
     </row>
     <row r="235" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="3" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C235" s="1" t="s">
         <v>324</v>
@@ -6366,10 +6366,10 @@
     </row>
     <row r="236" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
       <c r="C236" s="1" t="s">
         <v>325</v>
@@ -6381,7 +6381,7 @@
     </row>
     <row r="237" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
-        <v>747</v>
+        <v>742</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>82</v>
@@ -6396,10 +6396,10 @@
     </row>
     <row r="238" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A238" s="3" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C238" s="1" t="s">
         <v>326</v>
@@ -6411,10 +6411,10 @@
     </row>
     <row r="239" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>327</v>
@@ -6426,10 +6426,10 @@
     </row>
     <row r="240" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C240" s="1" t="s">
         <v>328</v>
@@ -6441,10 +6441,10 @@
     </row>
     <row r="241" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>329</v>
@@ -6456,10 +6456,10 @@
     </row>
     <row r="242" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>330</v>
@@ -6471,10 +6471,10 @@
     </row>
     <row r="243" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
-        <v>744</v>
+        <v>739</v>
       </c>
       <c r="B243" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C243" s="1" t="s">
         <v>331</v>
@@ -6486,10 +6486,10 @@
     </row>
     <row r="244" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A244" s="3" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="B244" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C244" s="1" t="s">
         <v>332</v>
@@ -6501,10 +6501,10 @@
     </row>
     <row r="245" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A245" s="3" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="B245" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C245" s="1" t="s">
         <v>333</v>
@@ -6516,10 +6516,10 @@
     </row>
     <row r="246" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" s="2" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="B246" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C246" s="1" t="s">
         <v>334</v>
@@ -6531,10 +6531,10 @@
     </row>
     <row r="247" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B247" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>335</v>
@@ -6546,10 +6546,10 @@
     </row>
     <row r="248" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="B248" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C248" s="1" t="s">
         <v>336</v>
@@ -6561,10 +6561,10 @@
     </row>
     <row r="249" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C249" s="1" t="s">
         <v>337</v>
@@ -6576,10 +6576,10 @@
     </row>
     <row r="250" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B250" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C250" s="1" t="s">
         <v>338</v>

</xml_diff>